<commit_message>
Cambios y actualización de bd
</commit_message>
<xml_diff>
--- a/storage/app/files/users.xlsx
+++ b/storage/app/files/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\gastceesto\storage\app\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EAE0CD-AC2B-48FC-86C5-39159056C6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3504B5E2-0520-4C4A-884F-4E68C367287A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{613FCEDD-3B0E-47B8-8AB3-82F656CF06BC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>jose.garcia.a@salud.qroo.gob.mx</t>
   </si>
@@ -99,6 +99,51 @@
   </si>
   <si>
     <t>jsoberanis</t>
+  </si>
+  <si>
+    <t>laralila.aguilar@salud.qroo.gob.mx</t>
+  </si>
+  <si>
+    <t>Laralila Aguilar</t>
+  </si>
+  <si>
+    <t>laguilar</t>
+  </si>
+  <si>
+    <t>ricardo.may@salud.qroo.gob.mx</t>
+  </si>
+  <si>
+    <t>Ricardo May</t>
+  </si>
+  <si>
+    <t>rmay</t>
+  </si>
+  <si>
+    <t>margarita.che@salud.qroo.gob.mx</t>
+  </si>
+  <si>
+    <t>Margarita Che</t>
+  </si>
+  <si>
+    <t>mche</t>
+  </si>
+  <si>
+    <t>veneralda.rosado@salud.qroo.gob.mx</t>
+  </si>
+  <si>
+    <t>Veneralda Rosado</t>
+  </si>
+  <si>
+    <t>vrosado</t>
+  </si>
+  <si>
+    <t>norman.angulo@salud.qroo.gob.m</t>
+  </si>
+  <si>
+    <t>Norman Angulo</t>
+  </si>
+  <si>
+    <t>nangulo</t>
   </si>
 </sst>
 </file>
@@ -148,7 +193,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -171,17 +216,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0D389B-0DE4-4CCB-AC02-5E9B8911D556}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,15 +618,15 @@
         <v>8</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D7" si="0">"\App\Models\User::factory()-&gt;create(["</f>
+        <f t="shared" ref="D3:D14" si="0">"\App\Models\User::factory()-&gt;create(["</f>
         <v>\App\Models\User::factory()-&gt;create([</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E7" si="1">"'name'=&gt;'"&amp;B3&amp;"','email'=&gt;'"&amp;A3&amp;"','password'=&gt;'"&amp;C3&amp;"'"</f>
+        <f t="shared" ref="E3:E8" si="1">"'name'=&gt;'"&amp;B3&amp;"','email'=&gt;'"&amp;A3&amp;"','password'=&gt;'"&amp;C3&amp;"'"</f>
         <v>'name'=&gt;'Andres Pinto','email'=&gt;'andres.pinto@salud.qroo.gob.mx','password'=&gt;'apinto'</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F7" si="2">D3&amp;E3&amp;"]);"</f>
+        <f t="shared" ref="F3:F8" si="2">D3&amp;E3&amp;"]);"</f>
         <v>\App\Models\User::factory()-&gt;create(['name'=&gt;'Andres Pinto','email'=&gt;'andres.pinto@salud.qroo.gob.mx','password'=&gt;'apinto']);</v>
       </c>
     </row>
@@ -657,6 +720,121 @@
       <c r="F7" t="str">
         <f t="shared" si="2"/>
         <v>\App\Models\User::factory()-&gt;create(['name'=&gt;'Jose Soberanis','email'=&gt;'jose.soberanis@salud.qroo.gob.mx','password'=&gt;'jsoberanis']);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>\App\Models\User::factory()-&gt;create([</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>'name'=&gt;'Laralila Aguilar','email'=&gt;'laralila.aguilar@salud.qroo.gob.mx','password'=&gt;'laguilar'</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>\App\Models\User::factory()-&gt;create(['name'=&gt;'Laralila Aguilar','email'=&gt;'laralila.aguilar@salud.qroo.gob.mx','password'=&gt;'laguilar']);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>\App\Models\User::factory()-&gt;create([</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" ref="E9:E14" si="3">"'name'=&gt;'"&amp;B9&amp;"','email'=&gt;'"&amp;A9&amp;"','password'=&gt;'"&amp;C9&amp;"'"</f>
+        <v>'name'=&gt;'Ricardo May','email'=&gt;'ricardo.may@salud.qroo.gob.mx','password'=&gt;'rmay'</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" ref="F9:F14" si="4">D9&amp;E9&amp;"]);"</f>
+        <v>\App\Models\User::factory()-&gt;create(['name'=&gt;'Ricardo May','email'=&gt;'ricardo.may@salud.qroo.gob.mx','password'=&gt;'rmay']);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>\App\Models\User::factory()-&gt;create([</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="3"/>
+        <v>'name'=&gt;'Margarita Che','email'=&gt;'margarita.che@salud.qroo.gob.mx','password'=&gt;'mche'</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="4"/>
+        <v>\App\Models\User::factory()-&gt;create(['name'=&gt;'Margarita Che','email'=&gt;'margarita.che@salud.qroo.gob.mx','password'=&gt;'mche']);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>\App\Models\User::factory()-&gt;create([</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="3"/>
+        <v>'name'=&gt;'Veneralda Rosado','email'=&gt;'veneralda.rosado@salud.qroo.gob.mx','password'=&gt;'vrosado'</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="4"/>
+        <v>\App\Models\User::factory()-&gt;create(['name'=&gt;'Veneralda Rosado','email'=&gt;'veneralda.rosado@salud.qroo.gob.mx','password'=&gt;'vrosado']);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>\App\Models\User::factory()-&gt;create([</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="3"/>
+        <v>'name'=&gt;'Norman Angulo','email'=&gt;'norman.angulo@salud.qroo.gob.m','password'=&gt;'nangulo'</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="4"/>
+        <v>\App\Models\User::factory()-&gt;create(['name'=&gt;'Norman Angulo','email'=&gt;'norman.angulo@salud.qroo.gob.m','password'=&gt;'nangulo']);</v>
       </c>
     </row>
   </sheetData>
@@ -664,6 +842,6 @@
     <hyperlink ref="A5" r:id="rId1" xr:uid="{CFF499FE-7EBA-4B25-9E6C-60FAAE702F51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrego un usuario
</commit_message>
<xml_diff>
--- a/storage/app/files/users.xlsx
+++ b/storage/app/files/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\gastceesto\storage\app\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3504B5E2-0520-4C4A-884F-4E68C367287A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B210E9-DD3C-4D38-8BBD-9B73CD230CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{613FCEDD-3B0E-47B8-8AB3-82F656CF06BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{613FCEDD-3B0E-47B8-8AB3-82F656CF06BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>jose.garcia.a@salud.qroo.gob.mx</t>
   </si>
@@ -137,20 +137,29 @@
     <t>vrosado</t>
   </si>
   <si>
-    <t>norman.angulo@salud.qroo.gob.m</t>
-  </si>
-  <si>
     <t>Norman Angulo</t>
   </si>
   <si>
     <t>nangulo</t>
+  </si>
+  <si>
+    <t>norman.angulo@salud.qroo.gob.mx</t>
+  </si>
+  <si>
+    <t>jorge.castillo.al@salud.qroo.gob.mx</t>
+  </si>
+  <si>
+    <t>Jorge Castillo</t>
+  </si>
+  <si>
+    <t>jcastillo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +180,14 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -228,10 +245,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -246,8 +264,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,15 +580,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0D389B-0DE4-4CCB-AC02-5E9B8911D556}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F2" sqref="F2:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
   </cols>
@@ -618,7 +638,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D14" si="0">"\App\Models\User::factory()-&gt;create(["</f>
+        <f t="shared" ref="D3:D13" si="0">"\App\Models\User::factory()-&gt;create(["</f>
         <v>\App\Models\User::factory()-&gt;create([</v>
       </c>
       <c r="E3" t="str">
@@ -760,11 +780,11 @@
         <v>\App\Models\User::factory()-&gt;create([</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" ref="E9:E14" si="3">"'name'=&gt;'"&amp;B9&amp;"','email'=&gt;'"&amp;A9&amp;"','password'=&gt;'"&amp;C9&amp;"'"</f>
+        <f t="shared" ref="E9:E13" si="3">"'name'=&gt;'"&amp;B9&amp;"','email'=&gt;'"&amp;A9&amp;"','password'=&gt;'"&amp;C9&amp;"'"</f>
         <v>'name'=&gt;'Ricardo May','email'=&gt;'ricardo.may@salud.qroo.gob.mx','password'=&gt;'rmay'</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" ref="F9:F14" si="4">D9&amp;E9&amp;"]);"</f>
+        <f t="shared" ref="F9:F12" si="4">D9&amp;E9&amp;"]);"</f>
         <v>\App\Models\User::factory()-&gt;create(['name'=&gt;'Ricardo May','email'=&gt;'ricardo.may@salud.qroo.gob.mx','password'=&gt;'rmay']);</v>
       </c>
     </row>
@@ -815,14 +835,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -830,18 +850,43 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="3"/>
-        <v>'name'=&gt;'Norman Angulo','email'=&gt;'norman.angulo@salud.qroo.gob.m','password'=&gt;'nangulo'</v>
+        <v>'name'=&gt;'Norman Angulo','email'=&gt;'norman.angulo@salud.qroo.gob.mx','password'=&gt;'nangulo'</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="4"/>
-        <v>\App\Models\User::factory()-&gt;create(['name'=&gt;'Norman Angulo','email'=&gt;'norman.angulo@salud.qroo.gob.m','password'=&gt;'nangulo']);</v>
+        <v>\App\Models\User::factory()-&gt;create(['name'=&gt;'Norman Angulo','email'=&gt;'norman.angulo@salud.qroo.gob.mx','password'=&gt;'nangulo']);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>\App\Models\User::factory()-&gt;create([</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" ref="E13" si="5">"'name'=&gt;'"&amp;B13&amp;"','email'=&gt;'"&amp;A13&amp;"','password'=&gt;'"&amp;C13&amp;"'"</f>
+        <v>'name'=&gt;'Jorge Castillo','email'=&gt;'jorge.castillo.al@salud.qroo.gob.mx','password'=&gt;'jcastillo'</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" ref="F13" si="6">D13&amp;E13&amp;"]);"</f>
+        <v>\App\Models\User::factory()-&gt;create(['name'=&gt;'Jorge Castillo','email'=&gt;'jorge.castillo.al@salud.qroo.gob.mx','password'=&gt;'jcastillo']);</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A5" r:id="rId1" xr:uid="{CFF499FE-7EBA-4B25-9E6C-60FAAE702F51}"/>
+    <hyperlink ref="A12" r:id="rId2" xr:uid="{2E6E4B65-1190-48DE-A1C2-A4DBB7D2387E}"/>
+    <hyperlink ref="A13" r:id="rId3" xr:uid="{5795D067-277E-4DEF-91E9-45BE2CC560D7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>